<commit_message>
Esperienze fisica upload dati
</commit_message>
<xml_diff>
--- a/Es Intf/data/Calcolo Variabili.xlsx
+++ b/Es Intf/data/Calcolo Variabili.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berni\Desktop\Lab3\Es Intf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0396DFDD-29B3-4D9B-A44C-756651CD2038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE59DC82-206B-4B48-BB72-853C4B843B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>D [cm]</t>
   </si>
@@ -130,6 +131,21 @@
   </si>
   <si>
     <t>h25</t>
+  </si>
+  <si>
+    <t>sind</t>
+  </si>
+  <si>
+    <t>lambda [nm]</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Dv [um]</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -179,9 +195,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -197,6 +214,1041 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$J$3:$J$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>3.898966725235288E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1348315755636977E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5406244563092209E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6347559988484882E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5895785521947788E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10439875619889277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11220136578347477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11930744496759639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12605815267253351</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13211888018832249</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13782933875631756</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14319137190643835</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14854082533468396</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15354413192273184</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15853565693145202</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16351505613756948</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16782046430269801</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17244633613721014</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.17673160311788907</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.18100684351542606</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.18494413814480629</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1888725471196766</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.19279190927293063</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.19637657460603661</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.19995338336315777</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.20319810939005206</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$K$3:$K$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6DD8-4898-8112-94FA94EBC1A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="436420464"/>
+        <c:axId val="436420792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="436420464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436420792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="436420792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436420464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F339797B-EEDF-47E0-A001-977E2D172F47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +1553,9 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -533,6 +1588,13 @@
       <c r="I3" t="s">
         <v>1</v>
       </c>
+      <c r="J3">
+        <f>1/SQRT(1 + (B$2/F3)^2)</f>
+        <v>3.898966725235288E-2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F4">
@@ -548,6 +1610,13 @@
       <c r="I4" t="s">
         <v>5</v>
       </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J28" si="1">1/SQRT(1 + (B$2/F4)^2)</f>
+        <v>6.1348315755636977E-2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -564,6 +1633,13 @@
       <c r="I5" t="s">
         <v>12</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>7.5406244563092209E-2</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F6">
@@ -579,6 +1655,13 @@
       <c r="I6" t="s">
         <v>6</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>8.6347559988484882E-2</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F7">
@@ -594,6 +1677,13 @@
       <c r="I7" t="s">
         <v>7</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>9.5895785521947788E-2</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F8">
@@ -609,6 +1699,13 @@
       <c r="I8" t="s">
         <v>13</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0.10439875619889277</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F9">
@@ -624,6 +1721,13 @@
       <c r="I9" t="s">
         <v>14</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0.11220136578347477</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F10">
@@ -639,6 +1743,13 @@
       <c r="I10" t="s">
         <v>15</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0.11930744496759639</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F11">
@@ -654,6 +1765,13 @@
       <c r="I11" t="s">
         <v>16</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0.12605815267253351</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F12">
@@ -669,6 +1787,13 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0.13211888018832249</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F13">
@@ -684,6 +1809,13 @@
       <c r="I13" t="s">
         <v>17</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0.13782933875631756</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F14">
@@ -699,6 +1831,13 @@
       <c r="I14" t="s">
         <v>18</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.14319137190643835</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F15">
@@ -714,6 +1853,13 @@
       <c r="I15" t="s">
         <v>19</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0.14854082533468396</v>
+      </c>
+      <c r="K15">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F16">
@@ -729,8 +1875,15 @@
       <c r="I16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0.15354413192273184</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>46.5</v>
       </c>
@@ -744,8 +1897,15 @@
       <c r="I17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0.15853565693145202</v>
+      </c>
+      <c r="K17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>48</v>
       </c>
@@ -759,8 +1919,15 @@
       <c r="I18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0.16351505613756948</v>
+      </c>
+      <c r="K18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>49.3</v>
       </c>
@@ -774,8 +1941,15 @@
       <c r="I19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0.16782046430269801</v>
+      </c>
+      <c r="K19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>50.7</v>
       </c>
@@ -789,8 +1963,15 @@
       <c r="I20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0.17244633613721014</v>
+      </c>
+      <c r="K20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>52</v>
       </c>
@@ -804,8 +1985,15 @@
       <c r="I21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0.17673160311788907</v>
+      </c>
+      <c r="K21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>53.3</v>
       </c>
@@ -819,8 +2007,15 @@
       <c r="I22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0.18100684351542606</v>
+      </c>
+      <c r="K22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>54.5</v>
       </c>
@@ -834,8 +2029,15 @@
       <c r="I23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.18494413814480629</v>
+      </c>
+      <c r="K23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>55.7</v>
       </c>
@@ -849,8 +2051,15 @@
       <c r="I24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.1888725471196766</v>
+      </c>
+      <c r="K24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>56.9</v>
       </c>
@@ -864,8 +2073,15 @@
       <c r="I25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.19279190927293063</v>
+      </c>
+      <c r="K25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>58</v>
       </c>
@@ -879,8 +2095,15 @@
       <c r="I26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0.19637657460603661</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>59.1</v>
       </c>
@@ -894,8 +2117,15 @@
       <c r="I27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0.19995338336315777</v>
+      </c>
+      <c r="K27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>60.1</v>
       </c>
@@ -908,11 +2138,190 @@
       </c>
       <c r="I28" t="s">
         <v>31</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0.20319810939005206</v>
+      </c>
+      <c r="K28">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9516477-CD91-47AC-8E0F-6BFAD453E8B1}">
+  <dimension ref="B1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>632.79999999999995</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <f>C2/1000*B2/(2*D2)</f>
+        <v>0.21093333333333333</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2">
+        <v>50</v>
+      </c>
+      <c r="J2">
+        <f>2*E8*I2/H2</f>
+        <v>0.50092899999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>632.79999999999995</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <f>C3/1000*B3/(2*D3)</f>
+        <v>0.18079999999999999</v>
+      </c>
+      <c r="H3">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <f>2*E8*I3/H3</f>
+        <v>0.54154486486486486</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>632.79999999999995</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <f>C4/1000*B4/(2*D4)</f>
+        <v>0.22780799999999995</v>
+      </c>
+      <c r="H4">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+      <c r="J4">
+        <f>2*E8*I4/H4</f>
+        <v>0.53432426666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>632.79999999999995</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>120</v>
+      </c>
+      <c r="E5">
+        <f>C5/1000*B5/(2*D5)</f>
+        <v>0.18456666666666666</v>
+      </c>
+      <c r="H5">
+        <v>70</v>
+      </c>
+      <c r="I5">
+        <v>95</v>
+      </c>
+      <c r="J5">
+        <f>2*E8*I5/H5</f>
+        <v>0.5438657714285714</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>632.79999999999995</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>160</v>
+      </c>
+      <c r="E6" s="2">
+        <f>C6/1000*B6/(2*D6)</f>
+        <v>0.19775000000000001</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+      <c r="I6">
+        <v>130</v>
+      </c>
+      <c r="J6">
+        <f>2*E8*I6/H6</f>
+        <v>0.52622844444444439</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>AVERAGE(E2:E6)</f>
+        <v>0.20037159999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>